<commit_message>
UAT configuration & Permission tweaks
</commit_message>
<xml_diff>
--- a/AdtonesAdminWebApi/PromotionalUserCSV/testPromoUser.xlsx
+++ b/AdtonesAdminWebApi/PromotionalUserCSV/testPromoUser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdec2b537cbdbd80/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DC61019-0511-44E8-A853-7B5E4F5872AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{9DC61019-0511-44E8-A853-7B5E4F5872AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6402B855-BA56-4B2A-A3FF-01E27D5EB44A}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="3348" windowWidth="17280" windowHeight="8964" xr2:uid="{1EAAC383-775A-433A-BE2E-C4684E4254B3}"/>
+    <workbookView xWindow="1764" yWindow="1752" windowWidth="12240" windowHeight="6252" xr2:uid="{1EAAC383-775A-433A-BE2E-C4684E4254B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,34 +382,34 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>8888888</v>
+        <v>88888881</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>99999999</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7777777</v>
+        <v>77777771</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>666666</v>
+        <v>6666661</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5555555</v>
+        <v>55555551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished bug fixes 119
</commit_message>
<xml_diff>
--- a/AdtonesAdminWebApi/PromotionalUserCSV/testPromoUser.xlsx
+++ b/AdtonesAdminWebApi/PromotionalUserCSV/testPromoUser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdec2b537cbdbd80/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{9DC61019-0511-44E8-A853-7B5E4F5872AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6402B855-BA56-4B2A-A3FF-01E27D5EB44A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{9DC61019-0511-44E8-A853-7B5E4F5872AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F27ED403-56E0-409D-959C-AF579E660CC2}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="1752" windowWidth="12240" windowHeight="6252" xr2:uid="{1EAAC383-775A-433A-BE2E-C4684E4254B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EAAC383-775A-433A-BE2E-C4684E4254B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,34 +382,37 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>88888881</v>
+        <v>1111111111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>9999999</v>
+        <v>222222222</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>77777771</v>
+        <v>333333</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>6666661</v>
+        <v>4444444</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>55555551</v>
+        <v>5555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>